<commit_message>
arrange added trained model with tests video annotation
</commit_message>
<xml_diff>
--- a/Comparaison/compareHMM.xlsx
+++ b/Comparaison/compareHMM.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Iteration_var" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Iteration_var_25" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,10 +463,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>24874.89937018291</v>
+        <v>18427.43551750997</v>
       </c>
     </row>
     <row r="3">
@@ -477,10 +477,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D3" t="n">
-        <v>25246.87073485404</v>
+        <v>18484.18060407991</v>
       </c>
     </row>
     <row r="4">
@@ -491,10 +491,10 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D4" t="n">
-        <v>25247.46200786524</v>
+        <v>24287.8259956873</v>
       </c>
     </row>
     <row r="5">
@@ -505,10 +505,10 @@
         <v>30</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D5" t="n">
-        <v>25247.46200786524</v>
+        <v>24632.46639717198</v>
       </c>
     </row>
     <row r="6">
@@ -519,10 +519,10 @@
         <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>25247.46200786524</v>
+        <v>24632.46639717198</v>
       </c>
     </row>
     <row r="7">
@@ -533,10 +533,10 @@
         <v>50</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>25247.46200786541</v>
+        <v>24632.46639717198</v>
       </c>
     </row>
     <row r="8">
@@ -547,10 +547,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>30526.03773310802</v>
+        <v>30182.04691931459</v>
       </c>
     </row>
     <row r="9">
@@ -561,10 +561,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>30599.65933814444</v>
+        <v>31093.69283092749</v>
       </c>
     </row>
     <row r="10">
@@ -575,10 +575,10 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D10" t="n">
-        <v>31085.92546984608</v>
+        <v>31455.17599071387</v>
       </c>
     </row>
     <row r="11">
@@ -589,10 +589,10 @@
         <v>30</v>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D11" t="n">
-        <v>31101.19744460631</v>
+        <v>31456.68664610427</v>
       </c>
     </row>
     <row r="12">
@@ -603,10 +603,10 @@
         <v>40</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D12" t="n">
-        <v>31101.19420772755</v>
+        <v>31456.68664610354</v>
       </c>
     </row>
     <row r="13">
@@ -617,10 +617,10 @@
         <v>50</v>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>31101.19420772755</v>
+        <v>31456.68664610427</v>
       </c>
     </row>
     <row r="14">
@@ -631,10 +631,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D14" t="n">
-        <v>29899.39734033415</v>
+        <v>32237.40414260582</v>
       </c>
     </row>
     <row r="15">
@@ -645,10 +645,10 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>29906.98763140058</v>
+        <v>32355.32347022226</v>
       </c>
     </row>
     <row r="16">
@@ -659,10 +659,10 @@
         <v>20</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>30443.27331164982</v>
+        <v>32355.01509909366</v>
       </c>
     </row>
     <row r="17">
@@ -673,10 +673,10 @@
         <v>30</v>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D17" t="n">
-        <v>30448.95303536349</v>
+        <v>32355.01509909366</v>
       </c>
     </row>
     <row r="18">
@@ -687,10 +687,10 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>30448.95303536349</v>
+        <v>32355.01509909366</v>
       </c>
     </row>
     <row r="19">
@@ -701,10 +701,10 @@
         <v>50</v>
       </c>
       <c r="C19" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D19" t="n">
-        <v>30448.95303536349</v>
+        <v>32355.01509909366</v>
       </c>
     </row>
     <row r="20">
@@ -715,10 +715,10 @@
         <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>29884.79930237068</v>
+        <v>34949.61208207608</v>
       </c>
     </row>
     <row r="21">
@@ -729,10 +729,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D21" t="n">
-        <v>33358.35093191348</v>
+        <v>35817.29912095716</v>
       </c>
     </row>
     <row r="22">
@@ -743,10 +743,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D22" t="n">
-        <v>35389.45747378896</v>
+        <v>35817.97243779732</v>
       </c>
     </row>
     <row r="23">
@@ -757,10 +757,10 @@
         <v>30</v>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D23" t="n">
-        <v>35398.59326861134</v>
+        <v>35817.97243779732</v>
       </c>
     </row>
     <row r="24">
@@ -771,10 +771,10 @@
         <v>40</v>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D24" t="n">
-        <v>35722.3225900504</v>
+        <v>35817.97243779732</v>
       </c>
     </row>
     <row r="25">
@@ -785,10 +785,10 @@
         <v>50</v>
       </c>
       <c r="C25" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>35943.99461195701</v>
+        <v>35817.97243779732</v>
       </c>
     </row>
     <row r="26">
@@ -799,10 +799,10 @@
         <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D26" t="n">
-        <v>30954.69563664972</v>
+        <v>34501.24430229516</v>
       </c>
     </row>
     <row r="27">
@@ -813,10 +813,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D27" t="n">
-        <v>34478.35204216684</v>
+        <v>35871.25562381666</v>
       </c>
     </row>
     <row r="28">
@@ -827,10 +827,10 @@
         <v>20</v>
       </c>
       <c r="C28" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D28" t="n">
-        <v>35382.60256688834</v>
+        <v>35931.01352537696</v>
       </c>
     </row>
     <row r="29">
@@ -841,10 +841,10 @@
         <v>30</v>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D29" t="n">
-        <v>36055.88744650663</v>
+        <v>35943.34499074162</v>
       </c>
     </row>
     <row r="30">
@@ -855,10 +855,10 @@
         <v>40</v>
       </c>
       <c r="C30" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D30" t="n">
-        <v>36653.77915470303</v>
+        <v>35943.34499074162</v>
       </c>
     </row>
     <row r="31">
@@ -869,10 +869,10 @@
         <v>50</v>
       </c>
       <c r="C31" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D31" t="n">
-        <v>36802.48708234125</v>
+        <v>35943.34499074162</v>
       </c>
     </row>
     <row r="32">
@@ -883,10 +883,10 @@
         <v>5</v>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D32" t="n">
-        <v>35102.184759425</v>
+        <v>41727.81711285443</v>
       </c>
     </row>
     <row r="33">
@@ -897,10 +897,10 @@
         <v>10</v>
       </c>
       <c r="C33" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D33" t="n">
-        <v>36430.49231170901</v>
+        <v>42913.62967592233</v>
       </c>
     </row>
     <row r="34">
@@ -911,10 +911,10 @@
         <v>20</v>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D34" t="n">
-        <v>38318.02827972229</v>
+        <v>43161.15138072416</v>
       </c>
     </row>
     <row r="35">
@@ -925,10 +925,10 @@
         <v>30</v>
       </c>
       <c r="C35" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D35" t="n">
-        <v>38678.8514476947</v>
+        <v>43169.51755512197</v>
       </c>
     </row>
     <row r="36">
@@ -939,10 +939,10 @@
         <v>40</v>
       </c>
       <c r="C36" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D36" t="n">
-        <v>38737.21806701802</v>
+        <v>43198.45699120492</v>
       </c>
     </row>
     <row r="37">
@@ -953,10 +953,10 @@
         <v>50</v>
       </c>
       <c r="C37" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D37" t="n">
-        <v>39203.05605970354</v>
+        <v>43200.19223347787</v>
       </c>
     </row>
     <row r="38">
@@ -967,10 +967,10 @@
         <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D38" t="n">
-        <v>33339.604099166</v>
+        <v>37797.22730860364</v>
       </c>
     </row>
     <row r="39">
@@ -981,10 +981,10 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D39" t="n">
-        <v>36394.31445615672</v>
+        <v>42293.99795449823</v>
       </c>
     </row>
     <row r="40">
@@ -995,10 +995,10 @@
         <v>20</v>
       </c>
       <c r="C40" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D40" t="n">
-        <v>39997.72599641241</v>
+        <v>42657.30167917375</v>
       </c>
     </row>
     <row r="41">
@@ -1009,10 +1009,10 @@
         <v>30</v>
       </c>
       <c r="C41" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D41" t="n">
-        <v>40113.04714949281</v>
+        <v>43110.49568090266</v>
       </c>
     </row>
     <row r="42">
@@ -1023,10 +1023,10 @@
         <v>40</v>
       </c>
       <c r="C42" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D42" t="n">
-        <v>40214.10096305406</v>
+        <v>43766.50933862592</v>
       </c>
     </row>
     <row r="43">
@@ -1037,10 +1037,10 @@
         <v>50</v>
       </c>
       <c r="C43" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D43" t="n">
-        <v>40214.55290158071</v>
+        <v>44346.13751722303</v>
       </c>
     </row>
     <row r="44">
@@ -1051,10 +1051,10 @@
         <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D44" t="n">
-        <v>41586.61833340152</v>
+        <v>39875.76030790625</v>
       </c>
     </row>
     <row r="45">
@@ -1065,10 +1065,10 @@
         <v>10</v>
       </c>
       <c r="C45" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D45" t="n">
-        <v>42799.74934589899</v>
+        <v>42514.43132731086</v>
       </c>
     </row>
     <row r="46">
@@ -1079,10 +1079,10 @@
         <v>20</v>
       </c>
       <c r="C46" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D46" t="n">
-        <v>43942.70804712237</v>
+        <v>43841.83528409144</v>
       </c>
     </row>
     <row r="47">
@@ -1093,10 +1093,10 @@
         <v>30</v>
       </c>
       <c r="C47" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D47" t="n">
-        <v>45212.21169809745</v>
+        <v>43893.21098408449</v>
       </c>
     </row>
     <row r="48">
@@ -1107,10 +1107,10 @@
         <v>40</v>
       </c>
       <c r="C48" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D48" t="n">
-        <v>45279.51848589602</v>
+        <v>43916.15847872938</v>
       </c>
     </row>
     <row r="49">
@@ -1121,10 +1121,10 @@
         <v>50</v>
       </c>
       <c r="C49" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D49" t="n">
-        <v>45279.53956174848</v>
+        <v>43916.15847872938</v>
       </c>
     </row>
     <row r="50">
@@ -1135,10 +1135,10 @@
         <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D50" t="n">
-        <v>38958.72714786254</v>
+        <v>40025.38269902093</v>
       </c>
     </row>
     <row r="51">
@@ -1149,10 +1149,10 @@
         <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D51" t="n">
-        <v>45008.57512791597</v>
+        <v>42242.99836153993</v>
       </c>
     </row>
     <row r="52">
@@ -1163,10 +1163,10 @@
         <v>20</v>
       </c>
       <c r="C52" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D52" t="n">
-        <v>47785.53915948403</v>
+        <v>43117.54782147115</v>
       </c>
     </row>
     <row r="53">
@@ -1177,10 +1177,10 @@
         <v>30</v>
       </c>
       <c r="C53" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D53" t="n">
-        <v>47816.60748491399</v>
+        <v>43649.12175055363</v>
       </c>
     </row>
     <row r="54">
@@ -1191,10 +1191,10 @@
         <v>40</v>
       </c>
       <c r="C54" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D54" t="n">
-        <v>47856.32410119275</v>
+        <v>43651.52802864456</v>
       </c>
     </row>
     <row r="55">
@@ -1205,10 +1205,10 @@
         <v>50</v>
       </c>
       <c r="C55" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D55" t="n">
-        <v>47897.88773905914</v>
+        <v>43651.52802864456</v>
       </c>
     </row>
     <row r="56">
@@ -1219,10 +1219,10 @@
         <v>5</v>
       </c>
       <c r="C56" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D56" t="n">
-        <v>43356.98635654858</v>
+        <v>47894.98913304195</v>
       </c>
     </row>
     <row r="57">
@@ -1233,10 +1233,10 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D57" t="n">
-        <v>47158.58169598402</v>
+        <v>51287.94234083167</v>
       </c>
     </row>
     <row r="58">
@@ -1247,10 +1247,10 @@
         <v>20</v>
       </c>
       <c r="C58" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D58" t="n">
-        <v>50185.49317812778</v>
+        <v>51298.31170878369</v>
       </c>
     </row>
     <row r="59">
@@ -1261,10 +1261,10 @@
         <v>30</v>
       </c>
       <c r="C59" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D59" t="n">
-        <v>50631.8993630961</v>
+        <v>51298.31170878369</v>
       </c>
     </row>
     <row r="60">
@@ -1275,10 +1275,10 @@
         <v>40</v>
       </c>
       <c r="C60" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D60" t="n">
-        <v>52279.29166319887</v>
+        <v>51298.31170878369</v>
       </c>
     </row>
     <row r="61">
@@ -1289,10 +1289,10 @@
         <v>50</v>
       </c>
       <c r="C61" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D61" t="n">
-        <v>52279.29166319887</v>
+        <v>51298.31170878369</v>
       </c>
     </row>
     <row r="62">
@@ -1303,10 +1303,10 @@
         <v>5</v>
       </c>
       <c r="C62" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D62" t="n">
-        <v>45212.93340854663</v>
+        <v>44265.26480100225</v>
       </c>
     </row>
     <row r="63">
@@ -1317,10 +1317,10 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D63" t="n">
-        <v>51025.25051203692</v>
+        <v>47480.82274920973</v>
       </c>
     </row>
     <row r="64">
@@ -1331,10 +1331,10 @@
         <v>20</v>
       </c>
       <c r="C64" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D64" t="n">
-        <v>51595.87847578128</v>
+        <v>49774.98249483492</v>
       </c>
     </row>
     <row r="65">
@@ -1345,10 +1345,10 @@
         <v>30</v>
       </c>
       <c r="C65" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D65" t="n">
-        <v>51630.65617418992</v>
+        <v>49983.26834121739</v>
       </c>
     </row>
     <row r="66">
@@ -1359,10 +1359,10 @@
         <v>40</v>
       </c>
       <c r="C66" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D66" t="n">
-        <v>51630.65617418992</v>
+        <v>49983.26834121739</v>
       </c>
     </row>
     <row r="67">
@@ -1373,10 +1373,10 @@
         <v>50</v>
       </c>
       <c r="C67" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D67" t="n">
-        <v>51630.65617418992</v>
+        <v>49983.26834121739</v>
       </c>
     </row>
     <row r="68">
@@ -1387,10 +1387,10 @@
         <v>5</v>
       </c>
       <c r="C68" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D68" t="n">
-        <v>42476.68032022131</v>
+        <v>48659.56138390623</v>
       </c>
     </row>
     <row r="69">
@@ -1401,10 +1401,10 @@
         <v>10</v>
       </c>
       <c r="C69" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D69" t="n">
-        <v>44802.2382941883</v>
+        <v>52707.91177375704</v>
       </c>
     </row>
     <row r="70">
@@ -1415,10 +1415,10 @@
         <v>20</v>
       </c>
       <c r="C70" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D70" t="n">
-        <v>45839.10260391751</v>
+        <v>55130.31998579116</v>
       </c>
     </row>
     <row r="71">
@@ -1429,10 +1429,10 @@
         <v>30</v>
       </c>
       <c r="C71" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D71" t="n">
-        <v>46377.25595663898</v>
+        <v>55132.37388652727</v>
       </c>
     </row>
     <row r="72">
@@ -1443,10 +1443,10 @@
         <v>40</v>
       </c>
       <c r="C72" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D72" t="n">
-        <v>46377.25595663898</v>
+        <v>55392.18146926896</v>
       </c>
     </row>
     <row r="73">
@@ -1457,10 +1457,10 @@
         <v>50</v>
       </c>
       <c r="C73" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D73" t="n">
-        <v>46377.25595663898</v>
+        <v>56593.41472496915</v>
       </c>
     </row>
     <row r="74">
@@ -1471,10 +1471,10 @@
         <v>5</v>
       </c>
       <c r="C74" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D74" t="n">
-        <v>43694.58198705938</v>
+        <v>47572.14187778537</v>
       </c>
     </row>
     <row r="75">
@@ -1485,10 +1485,10 @@
         <v>10</v>
       </c>
       <c r="C75" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D75" t="n">
-        <v>46272.01585467851</v>
+        <v>52871.7998218869</v>
       </c>
     </row>
     <row r="76">
@@ -1499,10 +1499,10 @@
         <v>20</v>
       </c>
       <c r="C76" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D76" t="n">
-        <v>49738.31677676455</v>
+        <v>54666.45688543312</v>
       </c>
     </row>
     <row r="77">
@@ -1513,10 +1513,10 @@
         <v>30</v>
       </c>
       <c r="C77" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D77" t="n">
-        <v>50765.94217694097</v>
+        <v>54758.27046395944</v>
       </c>
     </row>
     <row r="78">
@@ -1527,10 +1527,10 @@
         <v>40</v>
       </c>
       <c r="C78" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D78" t="n">
-        <v>50837.12363346381</v>
+        <v>54758.2808366599</v>
       </c>
     </row>
     <row r="79">
@@ -1541,10 +1541,10 @@
         <v>50</v>
       </c>
       <c r="C79" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D79" t="n">
-        <v>50837.12956878557</v>
+        <v>54758.2808366599</v>
       </c>
     </row>
     <row r="80">
@@ -1555,10 +1555,10 @@
         <v>5</v>
       </c>
       <c r="C80" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D80" t="n">
-        <v>49039.85065182368</v>
+        <v>49338.93545778998</v>
       </c>
     </row>
     <row r="81">
@@ -1569,10 +1569,10 @@
         <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D81" t="n">
-        <v>52041.99018598861</v>
+        <v>49930.02998137043</v>
       </c>
     </row>
     <row r="82">
@@ -1583,10 +1583,10 @@
         <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D82" t="n">
-        <v>53311.9868507141</v>
+        <v>49930.02998137043</v>
       </c>
     </row>
     <row r="83">
@@ -1597,10 +1597,10 @@
         <v>30</v>
       </c>
       <c r="C83" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D83" t="n">
-        <v>53311.9868507141</v>
+        <v>49930.02998137043</v>
       </c>
     </row>
     <row r="84">
@@ -1611,10 +1611,10 @@
         <v>40</v>
       </c>
       <c r="C84" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D84" t="n">
-        <v>53311.9868507141</v>
+        <v>49930.02998137043</v>
       </c>
     </row>
     <row r="85">
@@ -1625,10 +1625,10 @@
         <v>50</v>
       </c>
       <c r="C85" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D85" t="n">
-        <v>53311.9868507141</v>
+        <v>49930.02998137043</v>
       </c>
     </row>
     <row r="86">
@@ -1639,10 +1639,10 @@
         <v>5</v>
       </c>
       <c r="C86" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D86" t="n">
-        <v>49911.71358943595</v>
+        <v>50249.86310425887</v>
       </c>
     </row>
     <row r="87">
@@ -1653,10 +1653,10 @@
         <v>10</v>
       </c>
       <c r="C87" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D87" t="n">
-        <v>52449.82264960548</v>
+        <v>52529.44933775962</v>
       </c>
     </row>
     <row r="88">
@@ -1667,10 +1667,10 @@
         <v>20</v>
       </c>
       <c r="C88" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D88" t="n">
-        <v>52449.82264960548</v>
+        <v>53731.52760518021</v>
       </c>
     </row>
     <row r="89">
@@ -1681,10 +1681,10 @@
         <v>30</v>
       </c>
       <c r="C89" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D89" t="n">
-        <v>52449.82264960548</v>
+        <v>55563.80997662534</v>
       </c>
     </row>
     <row r="90">
@@ -1695,10 +1695,10 @@
         <v>40</v>
       </c>
       <c r="C90" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D90" t="n">
-        <v>52449.82264960548</v>
+        <v>55888.5098518117</v>
       </c>
     </row>
     <row r="91">
@@ -1709,10 +1709,10 @@
         <v>50</v>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D91" t="n">
-        <v>52449.82264960548</v>
+        <v>55888.5098518117</v>
       </c>
     </row>
     <row r="92">
@@ -1723,10 +1723,10 @@
         <v>5</v>
       </c>
       <c r="C92" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D92" t="n">
-        <v>46839.44191348616</v>
+        <v>51231.89859001157</v>
       </c>
     </row>
     <row r="93">
@@ -1737,10 +1737,10 @@
         <v>10</v>
       </c>
       <c r="C93" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D93" t="n">
-        <v>53497.69131304323</v>
+        <v>58196.1169036862</v>
       </c>
     </row>
     <row r="94">
@@ -1751,10 +1751,10 @@
         <v>20</v>
       </c>
       <c r="C94" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D94" t="n">
-        <v>53751.94696286486</v>
+        <v>65834.20487540599</v>
       </c>
     </row>
     <row r="95">
@@ -1765,10 +1765,10 @@
         <v>30</v>
       </c>
       <c r="C95" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D95" t="n">
-        <v>53751.94696286486</v>
+        <v>67387.57690323798</v>
       </c>
     </row>
     <row r="96">
@@ -1779,10 +1779,10 @@
         <v>40</v>
       </c>
       <c r="C96" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D96" t="n">
-        <v>53751.94696286486</v>
+        <v>67446.31364213019</v>
       </c>
     </row>
     <row r="97">
@@ -1793,10 +1793,10 @@
         <v>50</v>
       </c>
       <c r="C97" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D97" t="n">
-        <v>53751.94696286486</v>
+        <v>67501.84614191701</v>
       </c>
     </row>
     <row r="98">
@@ -1807,10 +1807,10 @@
         <v>5</v>
       </c>
       <c r="C98" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D98" t="n">
-        <v>50354.46986283143</v>
+        <v>56045.58419837583</v>
       </c>
     </row>
     <row r="99">
@@ -1821,10 +1821,10 @@
         <v>10</v>
       </c>
       <c r="C99" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D99" t="n">
-        <v>58325.9080433931</v>
+        <v>58139.34085001307</v>
       </c>
     </row>
     <row r="100">
@@ -1835,10 +1835,10 @@
         <v>20</v>
       </c>
       <c r="C100" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D100" t="n">
-        <v>58687.29454626453</v>
+        <v>60344.48232061369</v>
       </c>
     </row>
     <row r="101">
@@ -1849,10 +1849,10 @@
         <v>30</v>
       </c>
       <c r="C101" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D101" t="n">
-        <v>58687.29454626453</v>
+        <v>60392.81865065631</v>
       </c>
     </row>
     <row r="102">
@@ -1863,10 +1863,10 @@
         <v>40</v>
       </c>
       <c r="C102" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D102" t="n">
-        <v>58687.29454626453</v>
+        <v>60931.53354867748</v>
       </c>
     </row>
     <row r="103">
@@ -1877,10 +1877,10 @@
         <v>50</v>
       </c>
       <c r="C103" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D103" t="n">
-        <v>58687.29454626453</v>
+        <v>60931.53354867748</v>
       </c>
     </row>
     <row r="104">
@@ -1891,10 +1891,10 @@
         <v>5</v>
       </c>
       <c r="C104" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D104" t="n">
-        <v>44459.78241757036</v>
+        <v>51623.3260592799</v>
       </c>
     </row>
     <row r="105">
@@ -1905,10 +1905,10 @@
         <v>10</v>
       </c>
       <c r="C105" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D105" t="n">
-        <v>48023.48908790915</v>
+        <v>50725.49962509537</v>
       </c>
     </row>
     <row r="106">
@@ -1919,10 +1919,10 @@
         <v>20</v>
       </c>
       <c r="C106" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D106" t="n">
-        <v>50941.26109597613</v>
+        <v>50725.49962509537</v>
       </c>
     </row>
     <row r="107">
@@ -1933,10 +1933,10 @@
         <v>30</v>
       </c>
       <c r="C107" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D107" t="n">
-        <v>50941.26109597613</v>
+        <v>50725.49962509537</v>
       </c>
     </row>
     <row r="108">
@@ -1947,10 +1947,10 @@
         <v>40</v>
       </c>
       <c r="C108" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D108" t="n">
-        <v>50941.26109597613</v>
+        <v>50725.49962509537</v>
       </c>
     </row>
     <row r="109">
@@ -1961,10 +1961,430 @@
         <v>50</v>
       </c>
       <c r="C109" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D109" t="n">
-        <v>50941.26109597613</v>
+        <v>50725.49962509537</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>20</v>
+      </c>
+      <c r="B110" t="n">
+        <v>5</v>
+      </c>
+      <c r="C110" t="n">
+        <v>30</v>
+      </c>
+      <c r="D110" t="n">
+        <v>51105.54266693773</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>20</v>
+      </c>
+      <c r="B111" t="n">
+        <v>10</v>
+      </c>
+      <c r="C111" t="n">
+        <v>30</v>
+      </c>
+      <c r="D111" t="n">
+        <v>58266.0621239062</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>20</v>
+      </c>
+      <c r="B112" t="n">
+        <v>20</v>
+      </c>
+      <c r="C112" t="n">
+        <v>30</v>
+      </c>
+      <c r="D112" t="n">
+        <v>60310.3765151858</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>20</v>
+      </c>
+      <c r="B113" t="n">
+        <v>30</v>
+      </c>
+      <c r="C113" t="n">
+        <v>30</v>
+      </c>
+      <c r="D113" t="n">
+        <v>60409.5435780535</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>20</v>
+      </c>
+      <c r="B114" t="n">
+        <v>40</v>
+      </c>
+      <c r="C114" t="n">
+        <v>30</v>
+      </c>
+      <c r="D114" t="n">
+        <v>60409.58181049659</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>20</v>
+      </c>
+      <c r="B115" t="n">
+        <v>50</v>
+      </c>
+      <c r="C115" t="n">
+        <v>30</v>
+      </c>
+      <c r="D115" t="n">
+        <v>60409.58181049659</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>21</v>
+      </c>
+      <c r="B116" t="n">
+        <v>5</v>
+      </c>
+      <c r="C116" t="n">
+        <v>30</v>
+      </c>
+      <c r="D116" t="n">
+        <v>57910.19803969796</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>21</v>
+      </c>
+      <c r="B117" t="n">
+        <v>10</v>
+      </c>
+      <c r="C117" t="n">
+        <v>30</v>
+      </c>
+      <c r="D117" t="n">
+        <v>60852.70493714912</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>21</v>
+      </c>
+      <c r="B118" t="n">
+        <v>20</v>
+      </c>
+      <c r="C118" t="n">
+        <v>30</v>
+      </c>
+      <c r="D118" t="n">
+        <v>61768.60706525504</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>21</v>
+      </c>
+      <c r="B119" t="n">
+        <v>30</v>
+      </c>
+      <c r="C119" t="n">
+        <v>30</v>
+      </c>
+      <c r="D119" t="n">
+        <v>61768.60706525504</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>21</v>
+      </c>
+      <c r="B120" t="n">
+        <v>40</v>
+      </c>
+      <c r="C120" t="n">
+        <v>30</v>
+      </c>
+      <c r="D120" t="n">
+        <v>61768.60706525504</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>21</v>
+      </c>
+      <c r="B121" t="n">
+        <v>50</v>
+      </c>
+      <c r="C121" t="n">
+        <v>30</v>
+      </c>
+      <c r="D121" t="n">
+        <v>61768.60706525504</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>22</v>
+      </c>
+      <c r="B122" t="n">
+        <v>5</v>
+      </c>
+      <c r="C122" t="n">
+        <v>30</v>
+      </c>
+      <c r="D122" t="n">
+        <v>51235.14767528558</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>22</v>
+      </c>
+      <c r="B123" t="n">
+        <v>10</v>
+      </c>
+      <c r="C123" t="n">
+        <v>30</v>
+      </c>
+      <c r="D123" t="n">
+        <v>60743.26714761237</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>22</v>
+      </c>
+      <c r="B124" t="n">
+        <v>20</v>
+      </c>
+      <c r="C124" t="n">
+        <v>30</v>
+      </c>
+      <c r="D124" t="n">
+        <v>65516.41516796206</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>22</v>
+      </c>
+      <c r="B125" t="n">
+        <v>30</v>
+      </c>
+      <c r="C125" t="n">
+        <v>30</v>
+      </c>
+      <c r="D125" t="n">
+        <v>65883.99246389919</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>22</v>
+      </c>
+      <c r="B126" t="n">
+        <v>40</v>
+      </c>
+      <c r="C126" t="n">
+        <v>30</v>
+      </c>
+      <c r="D126" t="n">
+        <v>67162.2518800808</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>22</v>
+      </c>
+      <c r="B127" t="n">
+        <v>50</v>
+      </c>
+      <c r="C127" t="n">
+        <v>30</v>
+      </c>
+      <c r="D127" t="n">
+        <v>67162.2518800808</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>23</v>
+      </c>
+      <c r="B128" t="n">
+        <v>5</v>
+      </c>
+      <c r="C128" t="n">
+        <v>30</v>
+      </c>
+      <c r="D128" t="n">
+        <v>53725.36907496131</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>23</v>
+      </c>
+      <c r="B129" t="n">
+        <v>10</v>
+      </c>
+      <c r="C129" t="n">
+        <v>30</v>
+      </c>
+      <c r="D129" t="n">
+        <v>58951.78657045706</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>23</v>
+      </c>
+      <c r="B130" t="n">
+        <v>20</v>
+      </c>
+      <c r="C130" t="n">
+        <v>30</v>
+      </c>
+      <c r="D130" t="n">
+        <v>67221.642702301</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>23</v>
+      </c>
+      <c r="B131" t="n">
+        <v>30</v>
+      </c>
+      <c r="C131" t="n">
+        <v>30</v>
+      </c>
+      <c r="D131" t="n">
+        <v>67225.98782532754</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>23</v>
+      </c>
+      <c r="B132" t="n">
+        <v>40</v>
+      </c>
+      <c r="C132" t="n">
+        <v>30</v>
+      </c>
+      <c r="D132" t="n">
+        <v>67225.98782532754</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>23</v>
+      </c>
+      <c r="B133" t="n">
+        <v>50</v>
+      </c>
+      <c r="C133" t="n">
+        <v>30</v>
+      </c>
+      <c r="D133" t="n">
+        <v>67225.98782532754</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>24</v>
+      </c>
+      <c r="B134" t="n">
+        <v>5</v>
+      </c>
+      <c r="C134" t="n">
+        <v>30</v>
+      </c>
+      <c r="D134" t="n">
+        <v>58345.68924133808</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>24</v>
+      </c>
+      <c r="B135" t="n">
+        <v>10</v>
+      </c>
+      <c r="C135" t="n">
+        <v>30</v>
+      </c>
+      <c r="D135" t="n">
+        <v>63377.61261505298</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>24</v>
+      </c>
+      <c r="B136" t="n">
+        <v>20</v>
+      </c>
+      <c r="C136" t="n">
+        <v>30</v>
+      </c>
+      <c r="D136" t="n">
+        <v>65068.748947295</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>24</v>
+      </c>
+      <c r="B137" t="n">
+        <v>30</v>
+      </c>
+      <c r="C137" t="n">
+        <v>30</v>
+      </c>
+      <c r="D137" t="n">
+        <v>65068.748947295</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>24</v>
+      </c>
+      <c r="B138" t="n">
+        <v>40</v>
+      </c>
+      <c r="C138" t="n">
+        <v>30</v>
+      </c>
+      <c r="D138" t="n">
+        <v>65068.748947295</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>24</v>
+      </c>
+      <c r="B139" t="n">
+        <v>50</v>
+      </c>
+      <c r="C139" t="n">
+        <v>30</v>
+      </c>
+      <c r="D139" t="n">
+        <v>65068.748947295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>